<commit_message>
sim of HepTh xlsx
</commit_message>
<xml_diff>
--- a/similarity-G_HepTh.xlsx
+++ b/similarity-G_HepTh.xlsx
@@ -348,7 +348,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,19 +365,16 @@
         <v>0.4813005509217758</v>
       </c>
       <c r="D1">
-        <v>-0.02048117615450479</v>
+        <v>-0.02042428036513438</v>
       </c>
       <c r="E1">
-        <v>-0.2838871527842421</v>
+        <v>-0.2823383113349731</v>
       </c>
       <c r="F1">
-        <v>-3.355919245401774E-05</v>
+        <v>-3.338007351689955E-05</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
       <c r="B2">
         <v>0.08510895396141298</v>
       </c>
@@ -385,13 +382,13 @@
         <v>0.0837288870758106</v>
       </c>
       <c r="D2">
-        <v>-0.04253052489129616</v>
+        <v>-0.04241237699940882</v>
       </c>
       <c r="E2">
-        <v>-0.04774878169187938</v>
+        <v>-0.04748827222003059</v>
       </c>
       <c r="F2">
-        <v>-0.05860300247868991</v>
+        <v>-0.05829021463284707</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -404,11 +401,17 @@
       <c r="C3">
         <v>0.4858982824915321</v>
       </c>
+      <c r="D3">
+        <v>-0.020236691044003</v>
+      </c>
+      <c r="E3">
+        <v>-0.2736187788046003</v>
+      </c>
+      <c r="F3">
+        <v>-3.243416007105181E-05</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
       <c r="B4">
         <v>0.08603536472388931</v>
       </c>
@@ -416,7 +419,13 @@
         <v>0.08452872606762506</v>
       </c>
       <c r="D4">
-        <v>-0.02015063465525713</v>
+        <v>-0.04202283529381859</v>
+      </c>
+      <c r="E4">
+        <v>-0.04602167871213612</v>
+      </c>
+      <c r="F4">
+        <v>-0.05663840587470741</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -430,27 +439,30 @@
         <v>0.4748258139579651</v>
       </c>
       <c r="D5">
-        <v>-0.04184413347728222</v>
+        <v>-0.02075516704708091</v>
       </c>
       <c r="E5">
-        <v>-0.2708897386602951</v>
+        <v>-0.2789229934737962</v>
+      </c>
+      <c r="F5">
+        <v>-3.298510209777308E-05</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
       <c r="B6">
         <v>0.08398114955492005</v>
       </c>
       <c r="C6">
         <v>0.082602517037276</v>
       </c>
+      <c r="D6">
+        <v>-0.04309948520826185</v>
+      </c>
       <c r="E6">
-        <v>-0.04556266413257239</v>
+        <v>-0.04691382823634792</v>
       </c>
       <c r="F6">
-        <v>-3.211859113669518E-05</v>
+        <v>-0.05760049270089667</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -464,16 +476,16 @@
         <v>0.7350350786882078</v>
       </c>
       <c r="D7">
-        <v>-0.02074846200134334</v>
+        <v>-0.025777836270233</v>
+      </c>
+      <c r="E7">
+        <v>-0.4024328803204771</v>
       </c>
       <c r="F7">
-        <v>-0.05608734115324134</v>
+        <v>-4.745086983336472E-05</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
       <c r="B8">
         <v>0.1296975067466871</v>
       </c>
@@ -481,7 +493,13 @@
         <v>0.1278695172535695</v>
       </c>
       <c r="D8">
-        <v>-0.04308556173470311</v>
+        <v>-0.0535293920068044</v>
+      </c>
+      <c r="E8">
+        <v>-0.06768773986282094</v>
+      </c>
+      <c r="F8">
+        <v>-0.08286145282759177</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -494,8 +512,14 @@
       <c r="C9">
         <v>0.7572264795203854</v>
       </c>
+      <c r="D9">
+        <v>-0.02692763198875292</v>
+      </c>
       <c r="E9">
-        <v>-0.2808032138347567</v>
+        <v>-0.3758758581391763</v>
+      </c>
+      <c r="F9">
+        <v>-4.438069385864546E-05</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -506,13 +530,19 @@
         <v>0.1317300183287769</v>
       </c>
       <c r="D10">
-        <v>-0.02588346600272223</v>
+        <v>-0.05591701931187308</v>
       </c>
       <c r="E10">
-        <v>-0.04723007443018805</v>
+        <v>-0.06322094577902851</v>
+      </c>
+      <c r="F10">
+        <v>-0.07750013400256306</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
       <c r="B11">
         <v>3242</v>
       </c>
@@ -520,10 +550,13 @@
         <v>0.740120608045582</v>
       </c>
       <c r="D11">
-        <v>-0.05374873917383251</v>
+        <v>-0.02792797929411883</v>
+      </c>
+      <c r="E11">
+        <v>-0.3806207792499032</v>
       </c>
       <c r="F11">
-        <v>-3.320254402687745E-05</v>
+        <v>-4.492923965179361E-05</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -533,11 +566,20 @@
       <c r="C12">
         <v>0.1287542154166379</v>
       </c>
+      <c r="D12">
+        <v>-0.05799430704426965</v>
+      </c>
+      <c r="E12">
+        <v>-0.06401902417052754</v>
+      </c>
       <c r="F12">
-        <v>-0.0579802023714358</v>
+        <v>-0.07845803638712082</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
       <c r="B13">
         <v>3542</v>
       </c>
@@ -545,10 +587,13 @@
         <v>0.8170570139455275</v>
       </c>
       <c r="D13">
-        <v>-0.02682443245287192</v>
+        <v>-0.02641307679014976</v>
       </c>
       <c r="E13">
-        <v>-0.4034428945289203</v>
+        <v>-0.486126745848356</v>
+      </c>
+      <c r="F13">
+        <v>-5.652978684547987E-05</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -559,18 +604,33 @@
         <v>0.1421383672304642</v>
       </c>
       <c r="D14">
-        <v>-0.05570271860978221</v>
+        <v>-0.05484851120877158</v>
       </c>
       <c r="E14">
-        <v>-0.06785762056179467</v>
+        <v>-0.08176474220282265</v>
+      </c>
+      <c r="F14">
+        <v>-0.09871558271745171</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
       <c r="B15">
         <v>3791</v>
       </c>
       <c r="C15">
         <v>0.8716184858934186</v>
+      </c>
+      <c r="D15">
+        <v>-0.02809375684972226</v>
+      </c>
+      <c r="E15">
+        <v>-0.4651478862989276</v>
+      </c>
+      <c r="F15">
+        <v>-5.434163712310543E-05</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -581,13 +641,19 @@
         <v>0.1516300898446721</v>
       </c>
       <c r="D16">
-        <v>-0.0278875087268442</v>
+        <v>-0.0583385551676109</v>
+      </c>
+      <c r="E16">
+        <v>-0.07823617468947844</v>
       </c>
       <c r="F16">
-        <v>-4.756763448173938E-05</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+        <v>-0.09489450913888584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
       <c r="B17">
         <v>3629</v>
       </c>
@@ -595,132 +661,30 @@
         <v>0.8333832667588545</v>
       </c>
       <c r="D17">
-        <v>-0.05791026721882925</v>
+        <v>-0.02878207076648515</v>
       </c>
       <c r="E17">
-        <v>-0.3742683699843115</v>
+        <v>-0.4283807008613367</v>
       </c>
       <c r="F17">
-        <v>-0.08306535400869139</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>-5.014859213172426E-05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="B18">
         <v>0.1461715068272445</v>
       </c>
       <c r="C18">
         <v>0.144978544694546</v>
       </c>
+      <c r="D18">
+        <v>-0.05976788480908614</v>
+      </c>
       <c r="E18">
-        <v>-0.06295057214561066</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="D19">
-        <v>-0.02647311072622743</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="D20">
-        <v>-0.05497317567107652</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="E21">
-        <v>-0.3821123531838566</v>
-      </c>
-      <c r="F21">
-        <v>-4.419485707773669E-05</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="D22">
-        <v>-0.02802246001291725</v>
-      </c>
-      <c r="E22">
-        <v>-0.06426990145557245</v>
-      </c>
-      <c r="F22">
-        <v>-0.07717561506942275</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="D23">
-        <v>-0.05819050254262827</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="D25">
-        <v>-0.02878389468875742</v>
-      </c>
-      <c r="E25">
-        <v>-0.4875397657667175</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="D26">
-        <v>-0.05977167230502951</v>
-      </c>
-      <c r="E26">
-        <v>-0.08200240698950427</v>
-      </c>
-      <c r="F26">
-        <v>-4.510167594473766E-05</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="F27">
-        <v>-0.07875915461327188</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="E29">
-        <v>-0.4637716276305834</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="E30">
-        <v>-0.07800469301071342</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="F31">
-        <v>-5.669333081751566E-05</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="F32">
-        <v>-0.09900117265861968</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6">
-      <c r="E33">
-        <v>-0.4269974573343678</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6">
-      <c r="E34">
-        <v>-0.07181941195043057</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6">
-      <c r="F36">
-        <v>-5.418242163625483E-05</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6">
-      <c r="F37">
-        <v>-0.09461647784885001</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6">
-      <c r="F41">
-        <v>-4.998858709679332E-05</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6">
-      <c r="F42">
-        <v>-0.08729296146066426</v>
+        <v>-0.07205206845689158</v>
+      </c>
+      <c r="F18">
+        <v>-0.08757237150521491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>